<commit_message>
CSVs up to date and a few minor changes
</commit_message>
<xml_diff>
--- a/Work/processed_results.xlsx
+++ b/Work/processed_results.xlsx
@@ -4,16 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="25620" windowHeight="17560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27980" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="results.csv" sheetId="1" r:id="rId2"/>
+    <sheet name="Data" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
-  <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId3"/>
-  </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="277">
   <si>
     <t>RMSE_Twitter</t>
   </si>
@@ -853,19 +849,7 @@
     <t>City</t>
   </si>
   <si>
-    <t>BEST</t>
-  </si>
-  <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
-    <t>Count of City</t>
-  </si>
-  <si>
-    <t>Total</t>
+    <t xml:space="preserve">Best </t>
   </si>
 </sst>
 </file>
@@ -922,13 +906,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -944,1997 +923,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Stefan Sabev" refreshedDate="40204.392431597225" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="272">
-  <cacheSource type="worksheet">
-    <worksheetSource name="Table1"/>
-  </cacheSource>
-  <cacheFields count="5">
-    <cacheField name="City" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="RMSE_Twitter" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.3599691973540899" maxValue="3335.8695251167001"/>
-    </cacheField>
-    <cacheField name="RMSE_L4F" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.44283258662114" maxValue="3160.0588597419501"/>
-    </cacheField>
-    <cacheField name="RMSE_Just_Twitter" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.8143622582451799" maxValue="5314.4125647024503"/>
-    </cacheField>
-    <cacheField name="BEST" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="2" count="2">
-        <n v="2"/>
-        <n v="1"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="272">
-  <r>
-    <s v="London"/>
-    <n v="3335.8695251167001"/>
-    <n v="3160.0588597419501"/>
-    <n v="5314.4125647024503"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Paris"/>
-    <n v="939.10572759105798"/>
-    <n v="921.67856378322006"/>
-    <n v="1462.87365631288"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Barcelona"/>
-    <n v="920.68310659728797"/>
-    <n v="897.64730973957205"/>
-    <n v="1374.34200702055"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Milan"/>
-    <n v="760.34365912205897"/>
-    <n v="760.92867180947405"/>
-    <n v="1081.54831809347"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Rome"/>
-    <n v="710.70525173514602"/>
-    <n v="705.83885105500804"/>
-    <n v="1061.26056426185"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Manchester"/>
-    <n v="574.84314223385798"/>
-    <n v="572.41162011383506"/>
-    <n v="755.20294538053997"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Dublin"/>
-    <n v="514.58423098452204"/>
-    <n v="527.88440903106505"/>
-    <n v="499.58076879119301"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Amsterdam"/>
-    <n v="550.22547807191199"/>
-    <n v="516.20545961240396"/>
-    <n v="985.76340594842998"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Tenerife"/>
-    <n v="544.61875287264797"/>
-    <n v="502.02707225691103"/>
-    <n v="817.30704236249301"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Moscow"/>
-    <n v="499.18032660008703"/>
-    <n v="495.21394064061599"/>
-    <n v="616.71104621963798"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Bangkok"/>
-    <n v="507.79060027591697"/>
-    <n v="493.75592269573298"/>
-    <n v="871.34219077982505"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Malaga"/>
-    <n v="484.55635688192399"/>
-    <n v="480.64562370976199"/>
-    <n v="677.68948592180004"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Berlin"/>
-    <n v="532.99336175334395"/>
-    <n v="478.282960030742"/>
-    <n v="856.28353566911596"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Istanbul"/>
-    <n v="449.69244809492602"/>
-    <n v="450.63894984809298"/>
-    <n v="577.03126721162801"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Madrid"/>
-    <n v="417.58543590411"/>
-    <n v="418.91212579659498"/>
-    <n v="571.98399403998201"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Alicante"/>
-    <n v="352.87809025409098"/>
-    <n v="347.28616591170697"/>
-    <n v="522.61852005085598"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Brussels"/>
-    <n v="338.76406240938599"/>
-    <n v="346.37067261266998"/>
-    <n v="371.19962214444001"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Edinburgh"/>
-    <n v="315.22477773833202"/>
-    <n v="304.26864008066599"/>
-    <n v="432.99925164986797"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Geneva"/>
-    <n v="274.30756031717499"/>
-    <n v="275.49501725739702"/>
-    <n v="587.928887638417"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Prague"/>
-    <n v="276.18800698686101"/>
-    <n v="256.31178754144702"/>
-    <n v="419.19691292112401"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Dubai"/>
-    <n v="236.89271628875301"/>
-    <n v="224.15959306588101"/>
-    <n v="423.20341996450998"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Lanzarote"/>
-    <n v="257.96246095517398"/>
-    <n v="223.802941867307"/>
-    <n v="400.08868540621501"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Stockholm"/>
-    <n v="218.545726353356"/>
-    <n v="221.71518072830401"/>
-    <n v="228.00068590831199"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Copenhagen"/>
-    <n v="229.696923320563"/>
-    <n v="215.82091228118799"/>
-    <n v="335.08789306094098"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Munich"/>
-    <n v="225.77673656202401"/>
-    <n v="212.180032841307"/>
-    <n v="331.09567956884001"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Frankfurt"/>
-    <n v="210.595007578859"/>
-    <n v="211.691124943413"/>
-    <n v="251.278219497431"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Oslo"/>
-    <n v="193.188722005778"/>
-    <n v="198.104369321402"/>
-    <n v="221.164813801017"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Delhi"/>
-    <n v="205.67655403277499"/>
-    <n v="196.99591312629099"/>
-    <n v="251.80625259656401"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Budapest"/>
-    <n v="191.903379837561"/>
-    <n v="195.40272320409599"/>
-    <n v="243.980902830491"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Glasgow"/>
-    <n v="202.42420284363399"/>
-    <n v="195.37415840903401"/>
-    <n v="303.59829949178999"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Dusseldorf"/>
-    <n v="192.50200344134899"/>
-    <n v="193.46381893154299"/>
-    <n v="229.31710826586601"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Venice"/>
-    <n v="205.21843624379699"/>
-    <n v="192.302992008904"/>
-    <n v="314.68562195982599"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Birmingham"/>
-    <n v="188.92024179585599"/>
-    <n v="189.74104822048301"/>
-    <n v="218.55154999358001"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Athens"/>
-    <n v="205.04654521576899"/>
-    <n v="186.911421341459"/>
-    <n v="384.07585379927002"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Belfast"/>
-    <n v="194.42445247046101"/>
-    <n v="182.698796651967"/>
-    <n v="263.28207399206298"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Bangalore"/>
-    <n v="153.73861632159699"/>
-    <n v="182.30916901178901"/>
-    <n v="164.58790931523799"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Lisbon"/>
-    <n v="191.06334518793"/>
-    <n v="172.215854031525"/>
-    <n v="303.12347049466899"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Orlando"/>
-    <n v="177.65229548075399"/>
-    <n v="170.53803565706099"/>
-    <n v="251.82994712861299"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Miami"/>
-    <n v="172.51058002773701"/>
-    <n v="161.012110479782"/>
-    <n v="300.63235732567398"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Tokyo"/>
-    <n v="183.872114409852"/>
-    <n v="155.698753592288"/>
-    <n v="211.919871342606"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Warsaw"/>
-    <n v="149.63428618457399"/>
-    <n v="152.28275356603501"/>
-    <n v="183.43169343580001"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Antalya"/>
-    <n v="151.850718599217"/>
-    <n v="149.929899805773"/>
-    <n v="202.669087609624"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Ibiza"/>
-    <n v="130.578419412616"/>
-    <n v="131.99836193258"/>
-    <n v="226.93651634533401"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Cancun"/>
-    <n v="138.839746764323"/>
-    <n v="128.86220370329301"/>
-    <n v="208.41677668851599"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Bristol"/>
-    <n v="130.09893429291199"/>
-    <n v="127.64638950948699"/>
-    <n v="168.55863276797101"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Liverpool"/>
-    <n v="124.58932215265099"/>
-    <n v="125.939402896484"/>
-    <n v="155.78336643889699"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Krakow"/>
-    <n v="121.031399636353"/>
-    <n v="123.15842285524801"/>
-    <n v="140.46296357199299"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Porto"/>
-    <n v="118.234117583543"/>
-    <n v="120.69579791614601"/>
-    <n v="140.37633164154201"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Nice"/>
-    <n v="149.16591807734599"/>
-    <n v="117.943867658599"/>
-    <n v="252.20563047911"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Vienna"/>
-    <n v="122.135235841396"/>
-    <n v="116.39881011072301"/>
-    <n v="200.12271445516399"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Nottingham"/>
-    <n v="111.571392086708"/>
-    <n v="113.20435771545699"/>
-    <n v="136.24874026350199"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Hamburg"/>
-    <n v="111.96767713910501"/>
-    <n v="108.44603472287601"/>
-    <n v="187.81080511233299"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Naples"/>
-    <n v="128.06576465119201"/>
-    <n v="102.736722541912"/>
-    <n v="191.91981461812301"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Zurich"/>
-    <n v="106.148474644942"/>
-    <n v="101.44619206562299"/>
-    <n v="196.68988311244499"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Chicago"/>
-    <n v="97.976573296838396"/>
-    <n v="98.866050066588699"/>
-    <n v="151.943511753704"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Phuket"/>
-    <n v="96.668699560854904"/>
-    <n v="98.794447275643904"/>
-    <n v="147.675578678927"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Chennai"/>
-    <n v="99.9754841596787"/>
-    <n v="97.168289902107404"/>
-    <n v="113.250333856178"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Pisa"/>
-    <n v="95.256360045731896"/>
-    <n v="96.870836511027093"/>
-    <n v="113.314726662501"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Cologne"/>
-    <n v="99.383143485116506"/>
-    <n v="95.756141673885494"/>
-    <n v="150.383321033676"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Sydney"/>
-    <n v="130.229952519363"/>
-    <n v="94.719206940628098"/>
-    <n v="180.55206673608001"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Valencia"/>
-    <n v="92.073443355923303"/>
-    <n v="93.369336894482501"/>
-    <n v="110.777793345823"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Bologna"/>
-    <n v="92.047493507149298"/>
-    <n v="93.223852954141407"/>
-    <n v="109.55446208149201"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Crete"/>
-    <n v="95.204018535031906"/>
-    <n v="91.502422361798196"/>
-    <n v="150.33773943731799"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Male"/>
-    <n v="102.505647876591"/>
-    <n v="89.677006770237497"/>
-    <n v="107.109294464494"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Catania"/>
-    <n v="99.921683159419601"/>
-    <n v="87.506760453121501"/>
-    <n v="152.870777078874"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Seville"/>
-    <n v="85.940569180374595"/>
-    <n v="87.296892071737602"/>
-    <n v="106.796906838555"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Mumbai"/>
-    <n v="100.399676009392"/>
-    <n v="85.085267074135203"/>
-    <n v="120.02517031835499"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Palermo"/>
-    <n v="75.511436571773103"/>
-    <n v="75.908392822938396"/>
-    <n v="111.892876852771"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Basel"/>
-    <n v="86.506928802676299"/>
-    <n v="75.1863451378793"/>
-    <n v="131.63628501063701"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Johannesburg"/>
-    <n v="85.345429310383494"/>
-    <n v="71.811041911286907"/>
-    <n v="119.719302241774"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Stuttgart"/>
-    <n v="76.943039963882796"/>
-    <n v="71.398698544484304"/>
-    <n v="120.515892698822"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Singapore"/>
-    <n v="86.327859020605104"/>
-    <n v="70.273355787622904"/>
-    <n v="130.21173296126199"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Helsinki"/>
-    <n v="70.464977317712695"/>
-    <n v="68.943861394894697"/>
-    <n v="95.289434813438206"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Hanoi"/>
-    <n v="86.472371835345299"/>
-    <n v="68.7815453502552"/>
-    <n v="134.80222250829101"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Newcastle"/>
-    <n v="75.955478798174994"/>
-    <n v="68.360859457508496"/>
-    <n v="113.810865426205"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Toronto"/>
-    <n v="70.184616959263806"/>
-    <n v="67.297729666529094"/>
-    <n v="109.954665498536"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Lyon"/>
-    <n v="70.506502084273095"/>
-    <n v="67.0636580120823"/>
-    <n v="106.689837404033"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Leeds"/>
-    <n v="65.972432849747193"/>
-    <n v="66.893475700894399"/>
-    <n v="61.654548372144802"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Havana"/>
-    <n v="65.351241804410606"/>
-    <n v="65.918088192555601"/>
-    <n v="167.38110697395501"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Melbourne"/>
-    <n v="81.218989382777906"/>
-    <n v="65.127869529281199"/>
-    <n v="116.211933039071"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Kiev"/>
-    <n v="73.616679249056105"/>
-    <n v="64.893924022207202"/>
-    <n v="97.480357315041104"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Lima"/>
-    <n v="71.480243417461594"/>
-    <n v="62.314604913911801"/>
-    <n v="104.15971596703299"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Ankara"/>
-    <n v="60.073987629000698"/>
-    <n v="62.118698953015603"/>
-    <n v="59.027313630497602"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Sochi"/>
-    <n v="67.443338435690706"/>
-    <n v="61.652003718451802"/>
-    <n v="74.302812996411404"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Seoul"/>
-    <n v="65.220074848969602"/>
-    <n v="60.902242759006199"/>
-    <n v="95.783548206386797"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Marseille"/>
-    <n v="59.3774185436219"/>
-    <n v="60.3262612240244"/>
-    <n v="71.543759727805096"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Boston"/>
-    <n v="60.303458153482502"/>
-    <n v="59.736561330690797"/>
-    <n v="86.411025410598299"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Bucharest"/>
-    <n v="70.014511090570593"/>
-    <n v="59.167007763552697"/>
-    <n v="103.886024894898"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Beijing"/>
-    <n v="62.481072590756298"/>
-    <n v="58.385443803031201"/>
-    <n v="97.002649865489701"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Sofia"/>
-    <n v="65.380168159728797"/>
-    <n v="57.983228758906499"/>
-    <n v="115.696694849282"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Shanghai"/>
-    <n v="56.706920347883496"/>
-    <n v="56.311748159413703"/>
-    <n v="75.580895065233406"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Manila"/>
-    <n v="67.801188073259496"/>
-    <n v="56.2991959226635"/>
-    <n v="101.246696944427"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Ahmedabad"/>
-    <n v="43.6092316885887"/>
-    <n v="53.257901047998999"/>
-    <n v="43.657653258946397"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Bari"/>
-    <n v="51.734760404526497"/>
-    <n v="52.594226156489803"/>
-    <n v="64.596036341041199"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Dallas"/>
-    <n v="54.697852868189003"/>
-    <n v="52.2144275762493"/>
-    <n v="83.361905262593993"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Washington"/>
-    <n v="52.351184884627799"/>
-    <n v="51.780536976893003"/>
-    <n v="68.020644614651602"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Riga"/>
-    <n v="49.172971704419403"/>
-    <n v="49.993312966297303"/>
-    <n v="47.004330071445601"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Honolulu"/>
-    <n v="55.975834388259301"/>
-    <n v="47.919342338895902"/>
-    <n v="75.037794507617406"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Auckland"/>
-    <n v="67.427706919773001"/>
-    <n v="47.177879431914903"/>
-    <n v="95.777644292026807"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Madeira"/>
-    <n v="54.231137559733199"/>
-    <n v="44.900668414161203"/>
-    <n v="89.226082919962806"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Toulouse"/>
-    <n v="49.863332907835698"/>
-    <n v="44.392229861940699"/>
-    <n v="71.491834159501494"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Vancouver"/>
-    <n v="50.356752655532901"/>
-    <n v="44.272504653218199"/>
-    <n v="74.782523449271693"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Novosibirsk"/>
-    <n v="42.930174338916103"/>
-    <n v="42.561263762685897"/>
-    <n v="49.686035895169802"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Bogota"/>
-    <n v="45.8249475375166"/>
-    <n v="42.3245151387557"/>
-    <n v="65.392560425101607"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Corfu"/>
-    <n v="43.057005978724803"/>
-    <n v="41.816026498405897"/>
-    <n v="69.480273763556099"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Aberdeen"/>
-    <n v="44.780345207067597"/>
-    <n v="41.793835577841897"/>
-    <n v="62.133417808079102"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Turin"/>
-    <n v="42.891546266215201"/>
-    <n v="41.660385167538799"/>
-    <n v="64.182774982522403"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Kolkata"/>
-    <n v="37.8102038212906"/>
-    <n v="39.901833387606402"/>
-    <n v="43.648795793333001"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Vilnius"/>
-    <n v="39.0682970428131"/>
-    <n v="39.671148751570399"/>
-    <n v="44.9310767342714"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Seattle"/>
-    <n v="42.411380256991798"/>
-    <n v="39.236527575128797"/>
-    <n v="66.642688850950194"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Bordeaux"/>
-    <n v="43.287033827036304"/>
-    <n v="39.1665250270215"/>
-    <n v="63.477110697779899"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Denver"/>
-    <n v="38.572360143468401"/>
-    <n v="38.069175144122099"/>
-    <n v="55.3726264962811"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Tirana"/>
-    <n v="50.803922547642301"/>
-    <n v="37.590525478758998"/>
-    <n v="71.801753350394407"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Southampton"/>
-    <n v="36.243943740547998"/>
-    <n v="37.272054196655901"/>
-    <n v="37.685051541169699"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Houston"/>
-    <n v="36.744079303138797"/>
-    <n v="37.169357468422596"/>
-    <n v="51.573462873045202"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Gothenburg"/>
-    <n v="36.499197800794001"/>
-    <n v="36.875060560576003"/>
-    <n v="41.725255771146799"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Jakarta"/>
-    <n v="41.147159858084002"/>
-    <n v="36.819276149237901"/>
-    <n v="59.359357429436599"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Jersey"/>
-    <n v="39.5804894197206"/>
-    <n v="36.757693987894399"/>
-    <n v="49.409217337240896"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Montreal"/>
-    <n v="35.9848318618387"/>
-    <n v="36.0629178418667"/>
-    <n v="47.744886488137503"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Bilbao"/>
-    <n v="42.624420552885802"/>
-    <n v="35.719904963156303"/>
-    <n v="64.126262076749398"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Bremen"/>
-    <n v="34.660568473159103"/>
-    <n v="35.538257419077397"/>
-    <n v="39.923676042074398"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Cork"/>
-    <n v="33.881959042771598"/>
-    <n v="34.967308633592602"/>
-    <n v="44.6609151194437"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Perth"/>
-    <n v="42.718015301756701"/>
-    <n v="34.337543859006999"/>
-    <n v="62.489348615205202"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Goa"/>
-    <n v="44.060567457546597"/>
-    <n v="34.301049126139603"/>
-    <n v="58.365967468105403"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Brisbane"/>
-    <n v="47.8864986143533"/>
-    <n v="33.729361781003803"/>
-    <n v="65.876586626914005"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Kathmandu"/>
-    <n v="43.532869050234197"/>
-    <n v="33.475002800597302"/>
-    <n v="53.162280393199097"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Beirut"/>
-    <n v="32.638838966756602"/>
-    <n v="32.7387742798375"/>
-    <n v="39.1690143213415"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Yerevan"/>
-    <n v="41.831324355213198"/>
-    <n v="31.960443550161699"/>
-    <n v="35.246328168397604"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Atlanta"/>
-    <n v="32.004911722339401"/>
-    <n v="31.538561637974301"/>
-    <n v="43.368289062870303"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Rhodes"/>
-    <n v="33.198441645387199"/>
-    <n v="31.075887650543901"/>
-    <n v="48.825492290490402"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Florence"/>
-    <n v="33.063063693694801"/>
-    <n v="30.4750876347575"/>
-    <n v="67.831038364586306"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Lahore"/>
-    <n v="42.889003037565999"/>
-    <n v="29.818656637310902"/>
-    <n v="47.590071303716101"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Taipei"/>
-    <n v="35.802034991828698"/>
-    <n v="29.7761355786811"/>
-    <n v="50.283838969926499"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Phoenix"/>
-    <n v="34.8519903597617"/>
-    <n v="28.867030701796399"/>
-    <n v="48.024197400490102"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Tampa"/>
-    <n v="30.973954026926801"/>
-    <n v="28.804526220183298"/>
-    <n v="43.8868176778684"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Verona"/>
-    <n v="28.239315368558"/>
-    <n v="27.628518658611199"/>
-    <n v="61.859118195468099"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Bergen"/>
-    <n v="27.748778624591299"/>
-    <n v="27.311763015932499"/>
-    <n v="35.9303841626311"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Guangzhou"/>
-    <n v="27.350576042477599"/>
-    <n v="27.0040318392813"/>
-    <n v="37.675086912801099"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Tallinn"/>
-    <n v="26.7788162436097"/>
-    <n v="26.929905095665202"/>
-    <n v="31.783547949764799"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Dubrovnik"/>
-    <n v="28.1627515262517"/>
-    <n v="26.494288753209801"/>
-    <n v="57.1387623767367"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Gibraltar"/>
-    <n v="26.553057116326698"/>
-    <n v="25.8967637939569"/>
-    <n v="50.409288972350602"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Cairo"/>
-    <n v="35.9688593837529"/>
-    <n v="25.745461045067199"/>
-    <n v="48.6034631637418"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Nuremberg"/>
-    <n v="24.8061199576569"/>
-    <n v="25.312022170228701"/>
-    <n v="28.1614006867133"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Gdansk"/>
-    <n v="24.2034706846161"/>
-    <n v="24.793237582205599"/>
-    <n v="26.497757738337501"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Inverness"/>
-    <n v="26.022506742196601"/>
-    <n v="24.573600496186"/>
-    <n v="35.509185210456899"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Zagreb"/>
-    <n v="30.604383410402601"/>
-    <n v="24.562057590456899"/>
-    <n v="44.020337140037398"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Doha"/>
-    <n v="25.925394967528401"/>
-    <n v="23.603010523431699"/>
-    <n v="36.106517838409403"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Mauritius"/>
-    <n v="26.929574974964702"/>
-    <n v="23.145943738341298"/>
-    <n v="39.509805833981602"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Innsbruck"/>
-    <n v="22.556729167659501"/>
-    <n v="22.587039233732099"/>
-    <n v="47.092218038389298"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Amman"/>
-    <n v="29.333560926243401"/>
-    <n v="22.286484132765299"/>
-    <n v="39.855439005846897"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Karachi"/>
-    <n v="32.195419432787901"/>
-    <n v="22.095014230503502"/>
-    <n v="35.8747225548206"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Nairobi"/>
-    <n v="30.871408334216401"/>
-    <n v="22.0447274788187"/>
-    <n v="47.162325823166697"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Minneapolis"/>
-    <n v="22.055287496991401"/>
-    <n v="21.978150754258699"/>
-    <n v="31.5173090344645"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Dortmund"/>
-    <n v="21.2166022743647"/>
-    <n v="21.821401368663398"/>
-    <n v="24.978399680399299"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Reus"/>
-    <n v="21.453552389878901"/>
-    <n v="21.751914261472699"/>
-    <n v="23.472450139913601"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Mykonos"/>
-    <n v="22.966448784645301"/>
-    <n v="21.593783382474399"/>
-    <n v="38.178808144272999"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Durban"/>
-    <n v="23.046866484999899"/>
-    <n v="20.4586832702851"/>
-    <n v="28.496894526707099"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Osaka"/>
-    <n v="25.441882805739802"/>
-    <n v="20.389530802501401"/>
-    <n v="35.273304023453797"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Nantes"/>
-    <n v="20.802249254919101"/>
-    <n v="20.3769449284083"/>
-    <n v="28.390848192877399"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Detroit"/>
-    <n v="20.672005864294"/>
-    <n v="20.265170718026699"/>
-    <n v="28.326367452425799"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Split"/>
-    <n v="20.413850500649499"/>
-    <n v="19.908701349487199"/>
-    <n v="41.873598014536498"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Dakar"/>
-    <n v="23.529132898216201"/>
-    <n v="19.755749284896499"/>
-    <n v="33.601461136587197"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Luxembourg"/>
-    <n v="23.047250041627599"/>
-    <n v="19.631497087196699"/>
-    <n v="34.230488030232799"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Sapporo"/>
-    <n v="23.3295726662231"/>
-    <n v="19.456636078726401"/>
-    <n v="36.854117443786002"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Calgary"/>
-    <n v="21.887045627359001"/>
-    <n v="19.341303825074601"/>
-    <n v="28.331770704718799"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Philadelphia"/>
-    <n v="20.075825957742101"/>
-    <n v="19.186198590292801"/>
-    <n v="29.8462991421565"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Grenoble"/>
-    <n v="22.150051488392599"/>
-    <n v="19.106740403484601"/>
-    <n v="37.238428465070101"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Poznan"/>
-    <n v="18.4106224086994"/>
-    <n v="18.975443138638202"/>
-    <n v="19.831937486708501"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Santander"/>
-    <n v="18.4818509374551"/>
-    <n v="18.892857955607699"/>
-    <n v="18.687787716177102"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Shannon"/>
-    <n v="18.511032807063501"/>
-    <n v="18.8490824353294"/>
-    <n v="18.525238491190201"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Kazan"/>
-    <n v="18.225355927103699"/>
-    <n v="18.386152947049698"/>
-    <n v="21.3232324724924"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Portland"/>
-    <n v="18.9154985768693"/>
-    <n v="18.271236590293"/>
-    <n v="26.590751764068301"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Austin"/>
-    <n v="18.5805237615652"/>
-    <n v="18.087578212047099"/>
-    <n v="25.485375141605299"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Hyderabad"/>
-    <n v="20.485853372368499"/>
-    <n v="18.031836962183501"/>
-    <n v="28.645756693518301"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Lagos"/>
-    <n v="24.3517050822947"/>
-    <n v="17.751092869931199"/>
-    <n v="29.438019876039199"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Lviv"/>
-    <n v="17.378666001588201"/>
-    <n v="17.659670073797599"/>
-    <n v="23.390568034930801"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Amritsar"/>
-    <n v="17.888744592971001"/>
-    <n v="16.7153699135302"/>
-    <n v="18.222224867137498"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Genoa"/>
-    <n v="17.6969142167329"/>
-    <n v="15.9896808670707"/>
-    <n v="24.4934930653184"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Guernsey"/>
-    <n v="16.399192582391301"/>
-    <n v="15.5836546826869"/>
-    <n v="21.446045175613701"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Knock"/>
-    <n v="15.1326080502126"/>
-    <n v="15.4228914841144"/>
-    <n v="14.0564423864221"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Kos"/>
-    <n v="16.320667454635199"/>
-    <n v="15.3870699964913"/>
-    <n v="24.7545859476906"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Salvador"/>
-    <n v="20.389844936063099"/>
-    <n v="15.0229403106357"/>
-    <n v="26.9779887885886"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Granada"/>
-    <n v="17.0708289814011"/>
-    <n v="14.4741502009085"/>
-    <n v="28.944465967794098"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Almeria"/>
-    <n v="15.526552670778401"/>
-    <n v="14.383813518888299"/>
-    <n v="21.111609509882999"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Okinawa"/>
-    <n v="16.243185860042001"/>
-    <n v="14.2338241523492"/>
-    <n v="19.7944017433285"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Perm"/>
-    <n v="14.452518798874999"/>
-    <n v="14.2272987192282"/>
-    <n v="18.6946788669099"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Cardiff"/>
-    <n v="14.2685364568552"/>
-    <n v="14.1301258568623"/>
-    <n v="17.145147975904099"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Baltimore"/>
-    <n v="14.9354528247123"/>
-    <n v="14.0856835392972"/>
-    <n v="19.579403074234701"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Busan"/>
-    <n v="16.658699642920201"/>
-    <n v="13.6174679251433"/>
-    <n v="22.275160332615599"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Rotterdam"/>
-    <n v="15.4479088978684"/>
-    <n v="13.389201303231699"/>
-    <n v="23.574249219050099"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Exeter"/>
-    <n v="13.17785642978"/>
-    <n v="13.374417492707099"/>
-    <n v="13.8333161734146"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Christchurch"/>
-    <n v="18.655687439025801"/>
-    <n v="13.154769901212401"/>
-    <n v="20.8250887027137"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Charlotte"/>
-    <n v="12.831838740143199"/>
-    <n v="12.9836226351034"/>
-    <n v="15.9945287899154"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Odessa"/>
-    <n v="15.0567438456301"/>
-    <n v="12.9160421271676"/>
-    <n v="16.2612546106403"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Leipzig"/>
-    <n v="12.241436369893799"/>
-    <n v="12.6331032639222"/>
-    <n v="13.9022277529458"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Oran"/>
-    <n v="12.342372756163201"/>
-    <n v="12.608834471542901"/>
-    <n v="13.9688430860948"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Tromso"/>
-    <n v="12.332723479877499"/>
-    <n v="12.6069202226396"/>
-    <n v="14.093405810348401"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Rabat"/>
-    <n v="12.056958283081"/>
-    <n v="12.402209403042701"/>
-    <n v="13.324778648356601"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Kuwait"/>
-    <n v="13.525323496385701"/>
-    <n v="12.352929036031499"/>
-    <n v="18.0340923851026"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Durham"/>
-    <n v="12.911535921226401"/>
-    <n v="12.003802882996901"/>
-    <n v="16.5489115731908"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Kingston"/>
-    <n v="12.8660246231176"/>
-    <n v="11.583370042369401"/>
-    <n v="15.474641976351201"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Cali"/>
-    <n v="12.883212585321001"/>
-    <n v="11.527717225152401"/>
-    <n v="15.9263640896403"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Riyadh"/>
-    <n v="12.2361059008641"/>
-    <n v="11.3138500044448"/>
-    <n v="15.9506981837408"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Medellin"/>
-    <n v="14.258138833986401"/>
-    <n v="11.2495072541662"/>
-    <n v="17.090558725044701"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Stavanger"/>
-    <n v="11.1482343413471"/>
-    <n v="11.108146049357"/>
-    <n v="13.7067180325239"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Nashville"/>
-    <n v="12.009994430949501"/>
-    <n v="10.8453166957341"/>
-    <n v="15.742963453203901"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Montpellier"/>
-    <n v="12.348502652659899"/>
-    <n v="10.6085492555623"/>
-    <n v="15.3146961793593"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Accra"/>
-    <n v="12.491237488521399"/>
-    <n v="10.062433946271399"/>
-    <n v="16.052336400401199"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Adelaide"/>
-    <n v="14.008197180541099"/>
-    <n v="10.042967784628001"/>
-    <n v="17.8952824855701"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Bournemouth"/>
-    <n v="9.6930266312429296"/>
-    <n v="9.83059245808324"/>
-    <n v="10.952369222739399"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Fukuoka"/>
-    <n v="13.574785701853299"/>
-    <n v="9.8283789942108992"/>
-    <n v="15.457191253605799"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Cebu"/>
-    <n v="10.4583526451454"/>
-    <n v="9.7206505994672501"/>
-    <n v="13.339109537632201"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Liberia"/>
-    <n v="11.526784135390299"/>
-    <n v="9.6342138715661108"/>
-    <n v="14.1142525603926"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Trieste"/>
-    <n v="10.255693341646399"/>
-    <n v="9.5238198340145601"/>
-    <n v="13.573772070571501"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Edmonton"/>
-    <n v="9.1684294524896703"/>
-    <n v="9.4812606168491804"/>
-    <n v="10.8050301581147"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Angeles"/>
-    <n v="9.7418585521947705"/>
-    <n v="8.9787069160662192"/>
-    <n v="11.813826448085701"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Newquay"/>
-    <n v="8.8533989428048407"/>
-    <n v="8.8986966958434603"/>
-    <n v="10.481931227116799"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Nassau"/>
-    <n v="10.0954548298327"/>
-    <n v="8.8252598567102591"/>
-    <n v="12.336239886093599"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Murmansk"/>
-    <n v="9.71821785877734"/>
-    <n v="8.7950658151208696"/>
-    <n v="11.767330067214999"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Pittsburgh"/>
-    <n v="8.5448602979501995"/>
-    <n v="8.7636440326367193"/>
-    <n v="10.408783372697799"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Ottawa"/>
-    <n v="8.8628122402703298"/>
-    <n v="8.5571702952283495"/>
-    <n v="9.4380375161189907"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Asturias"/>
-    <n v="10.15514129296"/>
-    <n v="8.4248128260422508"/>
-    <n v="11.512941380753601"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Lille"/>
-    <n v="7.7866404265239799"/>
-    <n v="8.03316233592877"/>
-    <n v="9.5180544168487007"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Dresden"/>
-    <n v="8.0015543576752606"/>
-    <n v="8.0055683745752795"/>
-    <n v="10.280842169103201"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Sacramento"/>
-    <n v="7.7673981376208703"/>
-    <n v="7.9391489807448199"/>
-    <n v="10.185097650785099"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Jacksonville"/>
-    <n v="8.2410269959405493"/>
-    <n v="7.8860593893469799"/>
-    <n v="10.6974618279057"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Bahrain"/>
-    <n v="8.0145027344425497"/>
-    <n v="7.6901057184890798"/>
-    <n v="11.008085593074901"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Indianapolis"/>
-    <n v="7.5171929461188203"/>
-    <n v="7.5077120605824597"/>
-    <n v="9.5601700286269704"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Zaragoza"/>
-    <n v="7.2345702650373402"/>
-    <n v="7.3078481258691399"/>
-    <n v="11.052901502081999"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Columbus"/>
-    <n v="7.1888619706479604"/>
-    <n v="7.27526334442741"/>
-    <n v="8.2525432053071004"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Recife"/>
-    <n v="9.6764796970308797"/>
-    <n v="7.2587987059737404"/>
-    <n v="11.9968545516167"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Kabul"/>
-    <n v="8.9363595982526292"/>
-    <n v="7.2565616858123603"/>
-    <n v="10.0540356617705"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Sanya"/>
-    <n v="6.8211460258207897"/>
-    <n v="7.2391895530242403"/>
-    <n v="6.5239355444775304"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Buffalo"/>
-    <n v="7.1958751506071499"/>
-    <n v="7.1874142135348702"/>
-    <n v="9.5598161492232006"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Almaty"/>
-    <n v="7.0129798701488797"/>
-    <n v="7.1740618523635797"/>
-    <n v="8.1377713003379899"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Cleveland"/>
-    <n v="6.8905082731706599"/>
-    <n v="7.0624974472425599"/>
-    <n v="6.9546940065069904"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Kerry"/>
-    <n v="6.863317772716"/>
-    <n v="6.8611836694664996"/>
-    <n v="8.5035156207799396"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Chengdu"/>
-    <n v="7.4117644082065199"/>
-    <n v="6.8554130072520101"/>
-    <n v="8.6505402820029094"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Albuquerque"/>
-    <n v="6.9618714249323803"/>
-    <n v="6.8070357408289697"/>
-    <n v="8.2458916264246298"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Nagoya"/>
-    <n v="7.0677318992733804"/>
-    <n v="6.4995058983800398"/>
-    <n v="8.5985916520237602"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Santiago"/>
-    <n v="6.7827194901459302"/>
-    <n v="6.3157270882968097"/>
-    <n v="8.1608524208030797"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Curacao"/>
-    <n v="6.5999270169879098"/>
-    <n v="6.23607872662103"/>
-    <n v="9.0083943119359908"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Anchorage"/>
-    <n v="6.6291946842122398"/>
-    <n v="6.1590743716393401"/>
-    <n v="8.11106289316883"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Monterrey"/>
-    <n v="5.9761887804474503"/>
-    <n v="6.1072604175433902"/>
-    <n v="6.9691229896454097"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Milwaukee"/>
-    <n v="5.77451137243066"/>
-    <n v="5.8142782639609898"/>
-    <n v="7.0320230950067399"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Halifax"/>
-    <n v="6.1468855240049196"/>
-    <n v="5.7795216231369597"/>
-    <n v="7.0925091876613902"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Winnipeg"/>
-    <n v="6.3362226809453901"/>
-    <n v="5.7485922189697796"/>
-    <n v="7.23483459205291"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Memphis"/>
-    <n v="6.6821639281204703"/>
-    <n v="5.7275372274920802"/>
-    <n v="7.2029691034421903"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Reno"/>
-    <n v="6.0157240863587198"/>
-    <n v="5.7117831144182798"/>
-    <n v="7.5547767909779697"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Doncaster"/>
-    <n v="6.35386661252201"/>
-    <n v="5.69428357079408"/>
-    <n v="7.7161852805244298"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="George"/>
-    <n v="6.8715651554616697"/>
-    <n v="5.68189770573718"/>
-    <n v="8.1733757826200701"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Brasilia"/>
-    <n v="5.6183131690845904"/>
-    <n v="5.4748906733025597"/>
-    <n v="6.7381732131540302"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Surabaya"/>
-    <n v="5.4287088295035399"/>
-    <n v="5.4591560350831303"/>
-    <n v="6.0562862712687497"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Alexandria"/>
-    <n v="7.3018511541209197"/>
-    <n v="5.3210223497138003"/>
-    <n v="7.9452698633431904"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Quebec"/>
-    <n v="5.1675927406880504"/>
-    <n v="5.0886903256898197"/>
-    <n v="6.0201439871880797"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Aarhus"/>
-    <n v="4.8045429292719097"/>
-    <n v="4.8605476108071404"/>
-    <n v="5.0428654522498899"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Wellington"/>
-    <n v="5.7256171623536796"/>
-    <n v="4.7980524895323597"/>
-    <n v="6.5073041388166999"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Kilimanjaro"/>
-    <n v="5.4708223655636097"/>
-    <n v="4.40808642854679"/>
-    <n v="6.70136576964721"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Astana"/>
-    <n v="4.8749798010308796"/>
-    <n v="4.3779709692610203"/>
-    <n v="6.2219147097288401"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Jerez"/>
-    <n v="4.2680895667428"/>
-    <n v="4.3546664846240102"/>
-    <n v="4.7697851575199302"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Curitiba"/>
-    <n v="5.1098852213961399"/>
-    <n v="4.1817345499390299"/>
-    <n v="5.6776159828457704"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Tijuana"/>
-    <n v="4.0858971846203502"/>
-    <n v="4.1197431538684697"/>
-    <n v="4.1842865281451296"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Boise"/>
-    <n v="3.94580809849217"/>
-    <n v="3.8729020375304701"/>
-    <n v="4.8903188178806296"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Hartford"/>
-    <n v="4.3358543507030003"/>
-    <n v="3.8197922063902801"/>
-    <n v="5.6569828170432697"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Munster"/>
-    <n v="3.8957798619723198"/>
-    <n v="3.77991847185175"/>
-    <n v="4.6776930225433002"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Baghdad"/>
-    <n v="4.0934010385641697"/>
-    <n v="3.2688241828617102"/>
-    <n v="4.4284338936493999"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Constantine"/>
-    <n v="3.2485427928909498"/>
-    <n v="3.1937190462145901"/>
-    <n v="3.7821369424518001"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Vigo"/>
-    <n v="3.7610943932469301"/>
-    <n v="3.1014187200252499"/>
-    <n v="4.4471334617799902"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Lourdes"/>
-    <n v="2.5630335353688598"/>
-    <n v="2.49471942310152"/>
-    <n v="3.02407782423164"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Waterford"/>
-    <n v="2.4696624342762998"/>
-    <n v="2.4170895960606398"/>
-    <n v="3.55719345601814"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Norwich"/>
-    <n v="2.3906031930536802"/>
-    <n v="2.3802644083895701"/>
-    <n v="2.8477571256827301"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Asuncion"/>
-    <n v="1.3599691973540899"/>
-    <n v="1.44283258662114"/>
-    <n v="2.8143622582451799"/>
-    <x v="1"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="A3:B7" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of City" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E273" totalsRowShown="0">
   <autoFilter ref="A1:E273"/>
-  <sortState ref="A2:D273">
+  <sortState ref="A2:E273">
     <sortCondition descending="1" ref="C1:C273"/>
   </sortState>
   <tableColumns count="5">
@@ -2942,11 +934,11 @@
     <tableColumn id="2" name="RMSE_Twitter"/>
     <tableColumn id="3" name="RMSE_L4F"/>
     <tableColumn id="4" name="RMSE_Just_Twitter"/>
-    <tableColumn id="5" name="BEST" dataDxfId="0">
+    <tableColumn id="5" name="Best " dataDxfId="0">
       <calculatedColumnFormula>IF(Table1[RMSE_Twitter]&lt;Table1[RMSE_L4F], 1, 2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3272,71 +1264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="B4" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="2">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="B7" s="3">
-        <v>272</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E273"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E11" sqref="A2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8261,7 +6192,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
Some more minor tweaks
</commit_message>
<xml_diff>
--- a/Work/processed_results.xlsx
+++ b/Work/processed_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="540" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -5455,7 +5455,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:B7" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" showAll="0">
@@ -6504,15 +6504,15 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D469" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D469" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D469"/>
   <sortState ref="A2:D469">
     <sortCondition descending="1" ref="C1:C469"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Place" dataDxfId="5"/>
-    <tableColumn id="2" name="RMSE_Twitter" dataDxfId="4"/>
-    <tableColumn id="3" name="RMSE_L4F" dataDxfId="3"/>
+    <tableColumn id="1" name="Place" dataDxfId="3"/>
+    <tableColumn id="2" name="RMSE_Twitter" dataDxfId="2"/>
+    <tableColumn id="3" name="RMSE_L4F" dataDxfId="1"/>
     <tableColumn id="4" name="Best" dataDxfId="0">
       <calculatedColumnFormula>IF(Table5[RMSE_Twitter]&lt;Table5[RMSE_L4F], 1, 2)</calculatedColumnFormula>
     </tableColumn>
@@ -28269,8 +28269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D469"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -35330,7 +35330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F469"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -44734,7 +44734,7 @@
   <dimension ref="A3:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="A4:B8"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>